<commit_message>
Finished set up of visulizations
</commit_message>
<xml_diff>
--- a/Data/Analysis_Food Hubs.xlsx
+++ b/Data/Analysis_Food Hubs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Projects\FoodHubs\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ta0jrg1\Documents\Projects\FoodHubs\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795F268F-9295-4077-835F-787058FABE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F07E86F-0C46-49D7-A242-472B63709470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{7FA3B4B5-9D15-B84A-A7DB-0A68A34FD98B}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="877">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="878">
   <si>
     <t>Hub Name</t>
   </si>
@@ -2680,9 +2680,6 @@
     <t>Prvt_Inst</t>
   </si>
   <si>
-    <t>Pub_Insti</t>
-  </si>
-  <si>
     <t>Farm_Scale</t>
   </si>
   <si>
@@ -2693,6 +2690,12 @@
   </si>
   <si>
     <t>Value_Add</t>
+  </si>
+  <si>
+    <t>Sale_Point</t>
+  </si>
+  <si>
+    <t>Pub_Inst</t>
   </si>
 </sst>
 </file>
@@ -17278,8 +17281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B59C92-0A90-4A23-B4F3-52F301A8F7BD}">
   <dimension ref="A1:AK13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AA21" sqref="AA21"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -17317,7 +17320,7 @@
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>219</v>
@@ -17350,7 +17353,7 @@
         <v>183</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>222</v>
+        <v>876</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>193</v>
@@ -17362,13 +17365,13 @@
         <v>871</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>872</v>
+        <v>877</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>40</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>202</v>
@@ -17389,16 +17392,16 @@
         <v>205</v>
       </c>
       <c r="Y1" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="Z1" s="2" t="s">
         <v>874</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>875</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>208</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="AD1" s="2" t="s">
         <v>16</v>

</xml_diff>